<commit_message>
Mango pending to review
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -465,22 +465,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3392</v>
+        <v>2657</v>
       </c>
       <c r="C2">
         <v>704</v>
       </c>
       <c r="D2">
-        <v>1044</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="G2">
-        <v>235</v>
+        <v>543</v>
       </c>
       <c r="H2">
         <v>743</v>
@@ -491,22 +491,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1319</v>
+        <v>1133</v>
       </c>
       <c r="C3">
         <v>343</v>
       </c>
       <c r="D3">
-        <v>339</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F3">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="G3">
-        <v>72</v>
+        <v>216</v>
       </c>
       <c r="H3">
         <v>273</v>
@@ -517,22 +517,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1731</v>
+        <v>1419</v>
       </c>
       <c r="C4">
         <v>258</v>
       </c>
       <c r="D4">
-        <v>375</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G4">
-        <v>57</v>
+        <v>120</v>
       </c>
       <c r="H4">
         <v>781</v>
@@ -543,22 +543,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>699</v>
+        <v>654</v>
       </c>
       <c r="C5">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="D5">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F5">
         <v>152</v>
       </c>
       <c r="G5">
-        <v>60</v>
+        <v>139</v>
       </c>
       <c r="H5">
         <v>113</v>
@@ -569,13 +569,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>624</v>
+        <v>499</v>
       </c>
       <c r="C6">
         <v>181</v>
       </c>
       <c r="D6">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="E6">
         <v>17</v>
@@ -584,7 +584,7 @@
         <v>89</v>
       </c>
       <c r="G6">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="H6">
         <v>169</v>
@@ -595,22 +595,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="C7">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
       <c r="F7">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G7">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H7">
         <v>66</v>
@@ -621,22 +621,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>682</v>
+        <v>647</v>
       </c>
       <c r="C8">
         <v>146</v>
       </c>
       <c r="D8">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="F8">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="G8">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="H8">
         <v>17</v>
@@ -647,25 +647,25 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>336</v>
+        <v>207</v>
       </c>
       <c r="C9">
         <v>43</v>
       </c>
       <c r="D9">
-        <v>133</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F9">
         <v>56</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -673,13 +673,13 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>607</v>
+        <v>616</v>
       </c>
       <c r="C10">
         <v>115</v>
       </c>
       <c r="D10">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="E10">
         <v>22</v>
@@ -688,7 +688,7 @@
         <v>339</v>
       </c>
       <c r="G10">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="H10">
         <v>60</v>
@@ -699,10 +699,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -714,7 +714,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="H11">
         <v>0</v>

</xml_diff>